<commit_message>
implement dense all action
</commit_message>
<xml_diff>
--- a/week2/dataset.xlsx
+++ b/week2/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yunlong\Desktop\Recommender-System\week2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC49FA8-6A4E-4FF4-9C9E-65C8D485B828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A9096C-8A78-439A-94FB-6BC1599DFFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2310" yWindow="2055" windowWidth="30420" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ml-1m</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -48,6 +48,22 @@
   </si>
   <si>
     <t>max seq len</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>retailrocket</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>retailrocket-remove view</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>actionnum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>filternum</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -373,20 +389,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="G7:L8"/>
+  <dimension ref="G7:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="F2" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
+    <col min="7" max="7" width="25.1640625" customWidth="1"/>
     <col min="10" max="10" width="13.08203125" customWidth="1"/>
     <col min="11" max="11" width="11.08203125" customWidth="1"/>
-    <col min="12" max="12" width="9.9140625" customWidth="1"/>
+    <col min="12" max="12" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="7:12">
+    <row r="7" spans="7:14">
       <c r="H7" t="s">
         <v>1</v>
       </c>
@@ -402,8 +419,14 @@
       <c r="L7" t="s">
         <v>5</v>
       </c>
+      <c r="M7" t="s">
+        <v>8</v>
+      </c>
+      <c r="N7" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="8" spans="7:12">
+    <row r="8" spans="7:14">
       <c r="G8" t="s">
         <v>0</v>
       </c>
@@ -421,6 +444,64 @@
       </c>
       <c r="L8">
         <v>2277</v>
+      </c>
+      <c r="M8">
+        <v>1000209</v>
+      </c>
+      <c r="N8">
+        <v>999611</v>
+      </c>
+    </row>
+    <row r="9" spans="7:14">
+      <c r="G9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9">
+        <v>75875</v>
+      </c>
+      <c r="I9">
+        <v>65712</v>
+      </c>
+      <c r="J9">
+        <v>11.59</v>
+      </c>
+      <c r="K9">
+        <v>5</v>
+      </c>
+      <c r="L9">
+        <v>7585</v>
+      </c>
+      <c r="M9">
+        <v>2756101</v>
+      </c>
+      <c r="N9">
+        <v>879086</v>
+      </c>
+    </row>
+    <row r="10" spans="7:14">
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10">
+        <v>1256</v>
+      </c>
+      <c r="I10">
+        <v>4205</v>
+      </c>
+      <c r="J10">
+        <v>15.18</v>
+      </c>
+      <c r="K10">
+        <v>5</v>
+      </c>
+      <c r="L10">
+        <v>866</v>
+      </c>
+      <c r="M10">
+        <v>91789</v>
+      </c>
+      <c r="N10">
+        <v>19067</v>
       </c>
     </row>
   </sheetData>

</xml_diff>